<commit_message>
feat : 튜토리얼 ping-pong 패턴 완
플레이어 이동 수치 조절
</commit_message>
<xml_diff>
--- a/DragAndDrop/Assets/06.Data/Excel/Tutorial/Tutorial_bitto_transform_excel.xlsx
+++ b/DragAndDrop/Assets/06.Data/Excel/Tutorial/Tutorial_bitto_transform_excel.xlsx
@@ -1,158 +1,152 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="HCell" lastEdited="13.0" lowestEdited="13.0" rupBuild="0.866"/>
+  <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82106\Downloads\"/>
+    <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.junheeStudy\Team_Project\idle\DragAndDrop\Assets\06.Data\Excel\Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F82395D9-7328-4DED-BAAA-360D6EC2088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3F7AF08-F6A3-4D5B-8A2F-91777CA3F740}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11445"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+  </x:sheets>
+  <x:calcPr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" mc:Ignorable="hs" hs:hclCalcId="904"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>action_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <x:si>
+    <x:t>action_num</x:t>
+  </x:si>
+  <x:si>
+    <x:t>duration</x:t>
+  </x:si>
+  <x:si>
+    <x:t>time</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+<x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fonts count="6">
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="맑은 고딕"/>
+      <x:sz val="11"/>
+      <x:color rgb="ff000000"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right>
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top>
+        <x:color auto="1"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="표준" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:dxfs/>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="0e2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="e8e8e8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="e97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="196b24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="0f9ed5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="a02b93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="4ea72e"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="96607d"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -325,21 +319,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -400,6 +394,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="20000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
     <a:lnDef>
       <a:spPr/>
       <a:bodyPr/>
@@ -419,77 +434,78 @@
         </a:fontRef>
       </a:style>
     </a:lnDef>
+    <a:txDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C9FF60-F986-4B5F-9019-49B76D892E73}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>29.5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>35.5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr codeName="Sheet1"/>
+  <x:dimension ref="A1:C4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <x:selection activeCell="O13" activeCellId="0" sqref="O13:O13"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
+  <x:cols>
+    <x:col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2">
+        <x:v>30.600000000000001</x:v>
+      </x:c>
+      <x:c r="B2">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C2">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3">
+        <x:v>35.5</x:v>
+      </x:c>
+      <x:c r="B3">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B4">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C4">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.69999998807907104492" right="0.69999998807907104492" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>
+  <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1"/>
+</x:worksheet>
 </file>
</xml_diff>